<commit_message>
Updating annotation files, finalizing annotations
</commit_message>
<xml_diff>
--- a/responses/2039/Holistic/features/all/anno_I01T_Holistic-2039.xlsx
+++ b/responses/2039/Holistic/features/all/anno_I01T_Holistic-2039.xlsx
@@ -1174,7 +1174,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4013,11 +4013,11 @@
         <v>0</v>
       </c>
       <c r="G98">
-        <f t="shared" ref="G98:G129" si="6">IF(OR(C98&lt;&gt;1,D98&lt;&gt;1, E98&lt;&gt;1, F98&lt;&gt;1), 0, 1)</f>
+        <f t="shared" ref="G98:G100" si="6">IF(OR(C98&lt;&gt;1,D98&lt;&gt;1, E98&lt;&gt;1, F98&lt;&gt;1), 0, 1)</f>
         <v>0</v>
       </c>
       <c r="H98">
-        <f t="shared" ref="H98:H129" si="7">IF(AND(B98=1, G98=1),3,IF(AND(B98=1, G98=0), 2, 1))</f>
+        <f t="shared" ref="H98:H100" si="7">IF(AND(B98=1, G98=1),3,IF(AND(B98=1, G98=0), 2, 1))</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>